<commit_message>
Part list and DC Motor
</commit_message>
<xml_diff>
--- a/Parts_List.xlsx
+++ b/Parts_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\RC-TANK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D9018C-8B21-4962-A906-D1FF4D85BFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADEFE5E-7EA3-4033-B846-5BB05C2B66BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Price [zł]</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Black Steel sheet 70mm x 10mm x 3mm</t>
+  </si>
+  <si>
+    <t>Heng long Sprocket wheel 1/16 RC Germany Tiger</t>
+  </si>
+  <si>
+    <t>Planetary gearbox for 540 Brushed Motor</t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,13 +492,31 @@
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>220</v>
+      </c>
+      <c r="C6">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>149.6</v>
+      </c>
+      <c r="C7">
+        <v>74.8</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>